<commit_message>
Submitted Version of Files
Sprint 1 submitted documentation
</commit_message>
<xml_diff>
--- a/TestPlanTracker.xlsx
+++ b/TestPlanTracker.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/storm/OtherGitProjects/CTRL-ALT-ELITE-CSCE-4901/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CodeProjects\4901Capstone\CTRL-ALT-ELITE-CSCE-4901\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AE2C23C-338E-AA49-BAD6-B8D1AF7B948F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B64CD268-C5ED-4BCE-9F53-51CE944890E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestPlan ScreenReader" sheetId="3" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Expected Outcome</t>
   </si>
@@ -74,9 +74,6 @@
   </si>
   <si>
     <t xml:space="preserve"> Trace to User Story ID and Name</t>
-  </si>
-  <si>
-    <t>Remove sample items before submitting this.</t>
   </si>
   <si>
     <t>1.Application is open</t>
@@ -269,6 +266,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -277,9 +277,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -695,44 +692,42 @@
   <dimension ref="A1:H32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.5" customWidth="1"/>
-    <col min="2" max="2" width="20.1640625" customWidth="1"/>
-    <col min="3" max="3" width="23.1640625" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" customWidth="1"/>
+    <col min="2" max="2" width="20.140625" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" customWidth="1"/>
     <col min="4" max="4" width="39" customWidth="1"/>
-    <col min="5" max="5" width="27.6640625" customWidth="1"/>
+    <col min="5" max="5" width="27.7109375" customWidth="1"/>
     <col min="6" max="6" width="16" customWidth="1"/>
-    <col min="7" max="7" width="17.33203125" customWidth="1"/>
-    <col min="8" max="8" width="17.6640625" customWidth="1"/>
+    <col min="7" max="7" width="17.28515625" customWidth="1"/>
+    <col min="8" max="8" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="20" x14ac:dyDescent="0.2">
-      <c r="A1" s="16" t="s">
+    <row r="1" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="A1" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
       <c r="D1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="17"/>
-      <c r="F1" s="18"/>
-    </row>
-    <row r="2" spans="1:8" ht="20" x14ac:dyDescent="0.2">
+      <c r="E1" s="18"/>
+      <c r="F1" s="19"/>
+    </row>
+    <row r="2" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A2" s="10"/>
-      <c r="B2" s="10" t="s">
-        <v>13</v>
-      </c>
+      <c r="B2" s="10"/>
       <c r="C2" s="10"/>
       <c r="D2" s="9"/>
       <c r="E2" s="11"/>
       <c r="F2" s="12"/>
     </row>
-    <row r="3" spans="1:8" s="8" customFormat="1" ht="29" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" s="8" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
@@ -758,48 +753,48 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="57" thickTop="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:8" ht="64.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>1</v>
       </c>
       <c r="B4" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="13" t="s">
-        <v>16</v>
-      </c>
       <c r="E4" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4" s="19"/>
+        <v>20</v>
+      </c>
+      <c r="F4" s="16"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:8" ht="28" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A5" s="4">
         <f>A4+1</f>
         <v>2</v>
       </c>
       <c r="B5" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="D5" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="E5" s="14" t="s">
         <v>19</v>
-      </c>
-      <c r="E5" s="14" t="s">
-        <v>20</v>
       </c>
       <c r="F5" s="15"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
         <f t="shared" ref="A6:A31" si="0">A5+1</f>
         <v>3</v>
@@ -812,7 +807,7 @@
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="4">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -825,7 +820,7 @@
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="4">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -838,7 +833,7 @@
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="4">
         <v>6</v>
       </c>
@@ -850,7 +845,7 @@
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="4">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -863,7 +858,7 @@
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
     </row>
-    <row r="11" spans="1:8" ht="28" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A11" s="4">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -877,7 +872,7 @@
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
     </row>
-    <row r="12" spans="1:8" ht="28" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A12" s="4">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -892,7 +887,7 @@
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
     </row>
-    <row r="13" spans="1:8" ht="42" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A13" s="4">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -907,7 +902,7 @@
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="4">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -920,7 +915,7 @@
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="4">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -933,7 +928,7 @@
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="4">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -946,7 +941,7 @@
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="4">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -959,7 +954,7 @@
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="4">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -972,7 +967,7 @@
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="4">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -985,7 +980,7 @@
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="4">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -998,7 +993,7 @@
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="4">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -1011,7 +1006,7 @@
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="4">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -1024,7 +1019,7 @@
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="4">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -1037,7 +1032,7 @@
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="4">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -1050,7 +1045,7 @@
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="4">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -1063,7 +1058,7 @@
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="4">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -1076,7 +1071,7 @@
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="4">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -1089,7 +1084,7 @@
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="4">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -1102,7 +1097,7 @@
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="4">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -1115,7 +1110,7 @@
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="4">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -1128,7 +1123,7 @@
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="4">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -1141,7 +1136,7 @@
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="4">
         <f>A31+1</f>
         <v>29</v>

</xml_diff>

<commit_message>
Test tracker for iOS
</commit_message>
<xml_diff>
--- a/TestPlanTracker.xlsx
+++ b/TestPlanTracker.xlsx
@@ -1,22 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27103"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CodeProjects\4901Capstone\CTRL-ALT-ELITE-CSCE-4901\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B64CD268-C5ED-4BCE-9F53-51CE944890E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C8B2FE12-11C6-4FEF-93B2-16FEEBFD0999}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestPlan ScreenReader" sheetId="3" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191028" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
@@ -33,26 +36,29 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
-  <si>
-    <t>Expected Outcome</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="57">
   <si>
     <t>Test Planner and Tracker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ProjectName </t>
   </si>
   <si>
     <t>Test 
 No. ID</t>
   </si>
   <si>
+    <t xml:space="preserve"> Trace to User Story ID and Name</t>
+  </si>
+  <si>
+    <t>Pre-conditions</t>
+  </si>
+  <si>
     <t xml:space="preserve">Test Description (steps) 
 </t>
   </si>
   <si>
-    <t>Pre-conditions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ProjectName </t>
+    <t>Expected Outcome</t>
   </si>
   <si>
     <t>Sprint 1Outcome</t>
@@ -62,25 +68,13 @@
   </si>
   <si>
     <t>Sprint 3 Outcome</t>
-  </si>
-  <si>
-    <t>Code red if it does not work</t>
-  </si>
-  <si>
-    <t>Code green if it passes completely</t>
-  </si>
-  <si>
-    <t>Code yellow if partially with note on issue</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Trace to User Story ID and Name</t>
-  </si>
-  <si>
-    <t>1.Application is open</t>
   </si>
   <si>
     <t>All screens accessable
 R10</t>
+  </si>
+  <si>
+    <t>1.Application is open</t>
   </si>
   <si>
     <t>1.Select an untested button on current screen
@@ -88,27 +82,165 @@
 3. Repeat till no untested buttons</t>
   </si>
   <si>
-    <t>Application opens to initial screen</t>
-  </si>
-  <si>
-    <t>1.Application is installed on IOS or Android device</t>
-  </si>
-  <si>
-    <t>1. Doubletap or otherwise open the application.</t>
-  </si>
-  <si>
-    <t>Initial screen is presented with no errors or crashes.</t>
-  </si>
-  <si>
     <t>Screens present:
 Home, login, chat, goals/emotion tracker, conversation history, settings, emotion history, profile</t>
+  </si>
+  <si>
+    <t>Application opens to initial screen (IOS</t>
+  </si>
+  <si>
+    <t>1.Application is installed on IOS</t>
+  </si>
+  <si>
+    <t>1. Doubletap or otherwise open the application.</t>
+  </si>
+  <si>
+    <t>Initial screen is presented with no errors or crashes.</t>
+  </si>
+  <si>
+    <t>iOS emulator is not working, we will test this in next sprint after fixing issues with emulator.</t>
+  </si>
+  <si>
+    <t>Application opens to initial screen (Android)</t>
+  </si>
+  <si>
+    <t>1.Application is installed on Andriod</t>
+  </si>
+  <si>
+    <t>Valid credentials for login R1 (IOS)</t>
+  </si>
+  <si>
+    <t>1. Application is installed on IOS
+2. Have a valid account</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.Launch app “MindLift” 
+2.Put in a valid username and password. 
+3.Click button that says “Login”. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">User should login and see homepage. </t>
+  </si>
+  <si>
+    <t>Valid credentials for login R1(Android)</t>
+  </si>
+  <si>
+    <t>1. Application is installed on android.
+2. Have a valid account</t>
+  </si>
+  <si>
+    <t>Deny Login with wrong credentials, R1 (IOS)</t>
+  </si>
+  <si>
+    <t>1. Application is installed on IOS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.Launch app “MindLift” 
+2.Put in a invalid username and password. 
+3.Click button that says “Login”. </t>
+  </si>
+  <si>
+    <t>User should be denied access and screen should give error.</t>
+  </si>
+  <si>
+    <t>Deny Login with wrong credentials, R1 (Android)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Application is installed on Android                       2. User should have a valid account    </t>
+  </si>
+  <si>
+    <t>Login without entering data, R1 (IOS)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.Launch app “MindLift” 
+2.Enter nothing 
+3.Click button that says “Login”. </t>
+  </si>
+  <si>
+    <t>Login without entering data, R1 (Android)</t>
+  </si>
+  <si>
+    <t>1. Application is installed on android</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Valid email, password and unique username signup success, R1 (IOS) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Launch app “MindLift” 
+2. Click on “Signup” 
+3. Put in a unique username and password.
+4. Click button that says “Signup”. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">User should be able to sign up and can is logged in using the credentials. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Valid email, password and unique username signup success, R1 (Android) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">User should be able to sign up and is logged in with credentials. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invalid password or a username that is not unique is entered to signup, R1 (IOS) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Launch app “MindLift” 
+2. Click on “Signup” 
+3. Put in a non-unique username or invalid password.
+4. Click button that says “Signup”. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Users should not be able to sign up and will receive errors.  </t>
+  </si>
+  <si>
+    <t>Invalid password or a username that is not unique is entered to signup R1 (Android)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Users is not able to sign up and is getting errors.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Either one or all sign up information boxes are left empty, R1 (IOS) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Launch app “MindLift” 
+2. Click on “Signup” 
+3. Put in a unique userna assword.
+4. Click button that says “Signup”. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">User should not be able to sign up and will receive error. </t>
+  </si>
+  <si>
+    <t>Either one or all sign up information boxes are left empty R1 (Android)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Launch app “MindLift” 
+2. Click on “Signup” 
+3. Leave one or both boxes blank
+4. Click button that says “Signup”. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify user lands on home screen once he/she logins, R1 (IOS) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.Login with valid email and password  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">User should land on home screen after logging in. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify user lands on home screen once he/she logins, R1 (Android) </t>
+  </si>
+  <si>
+    <t>1. Application is installed on Android
+2. Have a valid account</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -151,7 +283,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -161,6 +293,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -221,15 +365,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -269,6 +410,12 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -277,6 +424,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -692,10 +842,10 @@
   <dimension ref="A1:H32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="9.42578125" customWidth="1"/>
     <col min="2" max="2" width="20.140625" customWidth="1"/>
@@ -707,294 +857,409 @@
     <col min="8" max="8" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:8" ht="20.25">
+      <c r="A1" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="9" t="s">
+      <c r="E1" s="19"/>
+      <c r="F1" s="20"/>
+    </row>
+    <row r="2" spans="1:8" ht="20.25">
+      <c r="A2" s="9"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="11"/>
+    </row>
+    <row r="3" spans="1:8" s="7" customFormat="1" ht="26.25" thickBot="1">
+      <c r="A3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="18"/>
-      <c r="F1" s="19"/>
-    </row>
-    <row r="2" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A2" s="10"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="12"/>
-    </row>
-    <row r="3" spans="1:8" s="8" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="6" t="s">
+      <c r="E3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="64.5" thickTop="1">
+      <c r="A4" s="2">
+        <v>1</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="64.5" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="3">
-        <v>1</v>
-      </c>
-      <c r="B4" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="13" t="s">
+      <c r="E4" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" s="16"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-    </row>
-    <row r="5" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A5" s="4">
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="16"/>
+    </row>
+    <row r="5" spans="1:8" ht="84" customHeight="1">
+      <c r="A5" s="3">
         <f>A4+1</f>
         <v>2</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="E5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="F5" s="14"/>
+      <c r="G5" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="14" t="s">
+      <c r="H5" s="17"/>
+    </row>
+    <row r="6" spans="1:8" ht="24">
+      <c r="A6" s="3">
+        <f>A5+1</f>
+        <v>3</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="15"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="4">
-        <f t="shared" ref="A6:A31" si="0">A5+1</f>
-        <v>3</v>
-      </c>
-      <c r="B6" s="14"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="4">
-        <f t="shared" si="0"/>
+      <c r="C6" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="17"/>
+    </row>
+    <row r="7" spans="1:8" ht="36">
+      <c r="A7" s="3">
+        <f t="shared" ref="A6:A31" si="0">A6+1</f>
         <v>4</v>
       </c>
-      <c r="B7" s="14"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
+      <c r="B7" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>24</v>
+      </c>
       <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="4">
+      <c r="G7" s="21"/>
+      <c r="H7" s="17"/>
+    </row>
+    <row r="8" spans="1:8" ht="36">
+      <c r="A8" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B8" s="14"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
+      <c r="B8" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>24</v>
+      </c>
       <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="4">
+      <c r="G8" s="14"/>
+      <c r="H8" s="17"/>
+    </row>
+    <row r="9" spans="1:8" ht="36">
+      <c r="A9" s="3">
         <v>6</v>
       </c>
-      <c r="B9" s="14"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
+      <c r="B9" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>30</v>
+      </c>
       <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="4">
+      <c r="G9" s="21"/>
+      <c r="H9" s="17"/>
+    </row>
+    <row r="10" spans="1:8" ht="48">
+      <c r="A10" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
+      <c r="B10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-    </row>
-    <row r="11" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A11" s="4">
-        <f t="shared" si="0"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="17"/>
+    </row>
+    <row r="11" spans="1:8" ht="36">
+      <c r="A11" s="3">
         <v>8</v>
       </c>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="F11" s="1" t="s">
+      <c r="B11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F11" s="1"/>
+      <c r="G11" s="21"/>
+      <c r="H11" s="17"/>
+    </row>
+    <row r="12" spans="1:8" ht="36">
+      <c r="A12" s="3">
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-    </row>
-    <row r="12" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A12" s="4">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1" t="s">
+      <c r="B12" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F12" s="1"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="17"/>
+    </row>
+    <row r="13" spans="1:8" ht="48">
+      <c r="A13" s="3">
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-    </row>
-    <row r="13" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A13" s="4">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1" t="s">
+      <c r="B13" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F13" s="1"/>
+      <c r="G13" s="21"/>
+      <c r="H13" s="17"/>
+    </row>
+    <row r="14" spans="1:8" ht="48">
+      <c r="A14" s="3">
         <v>11</v>
       </c>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="4">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
+      <c r="B14" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>41</v>
+      </c>
       <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="4">
+      <c r="G14" s="15"/>
+      <c r="H14" s="17"/>
+    </row>
+    <row r="15" spans="1:8" ht="60">
+      <c r="A15" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
+      <c r="B15" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>44</v>
+      </c>
       <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="4">
+      <c r="G15" s="21"/>
+      <c r="H15" s="17"/>
+    </row>
+    <row r="16" spans="1:8" ht="48">
+      <c r="A16" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
+      <c r="B16" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A17" s="4">
+      <c r="G16" s="14"/>
+      <c r="H16" s="17"/>
+    </row>
+    <row r="17" spans="1:8" ht="48">
+      <c r="A17" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
+      <c r="B17" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A18" s="4">
+      <c r="G17" s="21"/>
+      <c r="H17" s="17"/>
+    </row>
+    <row r="18" spans="1:8" ht="48">
+      <c r="A18" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
+      <c r="B18" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A19" s="4">
+      <c r="G18" s="14"/>
+      <c r="H18" s="17"/>
+    </row>
+    <row r="19" spans="1:8" ht="55.5" customHeight="1">
+      <c r="A19" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
+      <c r="B19" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>54</v>
+      </c>
       <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A20" s="4">
-        <f t="shared" si="0"/>
+      <c r="G19" s="21"/>
+      <c r="H19" s="17"/>
+    </row>
+    <row r="20" spans="1:8" ht="48">
+      <c r="A20" s="3">
+        <f>A19+1</f>
         <v>17</v>
       </c>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
+      <c r="B20" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>54</v>
+      </c>
       <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A21" s="4">
+      <c r="G20" s="14"/>
+      <c r="H20" s="17"/>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" s="3">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
@@ -1006,8 +1271,8 @@
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A22" s="4">
+    <row r="22" spans="1:8">
+      <c r="A22" s="3">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
@@ -1019,8 +1284,8 @@
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A23" s="4">
+    <row r="23" spans="1:8">
+      <c r="A23" s="3">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
@@ -1032,8 +1297,8 @@
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A24" s="4">
+    <row r="24" spans="1:8">
+      <c r="A24" s="3">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
@@ -1045,8 +1310,8 @@
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A25" s="4">
+    <row r="25" spans="1:8">
+      <c r="A25" s="3">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
@@ -1058,8 +1323,8 @@
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A26" s="4">
+    <row r="26" spans="1:8">
+      <c r="A26" s="3">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
@@ -1071,8 +1336,8 @@
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A27" s="4">
+    <row r="27" spans="1:8">
+      <c r="A27" s="3">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
@@ -1084,8 +1349,8 @@
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A28" s="4">
+    <row r="28" spans="1:8">
+      <c r="A28" s="3">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
@@ -1097,8 +1362,8 @@
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A29" s="4">
+    <row r="29" spans="1:8">
+      <c r="A29" s="3">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
@@ -1110,8 +1375,8 @@
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A30" s="4">
+    <row r="30" spans="1:8">
+      <c r="A30" s="3">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
@@ -1123,8 +1388,8 @@
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A31" s="4">
+    <row r="31" spans="1:8">
+      <c r="A31" s="3">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
@@ -1136,8 +1401,8 @@
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A32" s="4">
+    <row r="32" spans="1:8">
+      <c r="A32" s="3">
         <f>A31+1</f>
         <v>29</v>
       </c>
@@ -1161,4 +1426,169 @@
     <oddHeader>&amp;R&amp;D</oddHeader>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010086172CFAA5FCEC4EBA8519FEE259A6B4" ma:contentTypeVersion="3" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2cf875f61f947313d43db5494becd2b8">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="34ab6044-38b2-4dc7-97bb-2eb507f60812" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2e11831833257d99d0be17644557580d" ns2:_="">
+    <xsd:import namespace="34ab6044-38b2-4dc7-97bb-2eb507f60812"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="34ab6044-38b2-4dc7-97bb-2eb507f60812" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="10" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{95C7F316-54F6-4CFB-856D-9AD09D022CA2}"/>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{20FD2E1A-4E2B-4A48-92AF-F21AB94E806B}"/>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{291DE61A-00D2-4874-9EE9-2262838A2644}"/>
 </file>
</xml_diff>

<commit_message>
updated tracker for iOS testing
</commit_message>
<xml_diff>
--- a/TestPlanTracker.xlsx
+++ b/TestPlanTracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CodeProjects\4901Capstone\CTRL-ALT-ELITE-CSCE-4901\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C8B2FE12-11C6-4FEF-93B2-16FEEBFD0999}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FCAA33AB-92E7-4006-A973-39725E78F57D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -240,7 +240,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -282,6 +282,11 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -304,7 +309,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -365,7 +370,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -424,6 +429,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -841,8 +849,8 @@
   </sheetPr>
   <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75"/>
@@ -941,7 +949,7 @@
         <v>17</v>
       </c>
       <c r="F5" s="14"/>
-      <c r="G5" s="21" t="s">
+      <c r="G5" s="22" t="s">
         <v>18</v>
       </c>
       <c r="H5" s="17"/>
@@ -985,7 +993,7 @@
         <v>24</v>
       </c>
       <c r="F7" s="1"/>
-      <c r="G7" s="21"/>
+      <c r="G7" s="22"/>
       <c r="H7" s="17"/>
     </row>
     <row r="8" spans="1:8" ht="36">
@@ -1067,7 +1075,7 @@
         <v>30</v>
       </c>
       <c r="F11" s="1"/>
-      <c r="G11" s="21"/>
+      <c r="G11" s="22"/>
       <c r="H11" s="17"/>
     </row>
     <row r="12" spans="1:8" ht="36">
@@ -1109,7 +1117,7 @@
         <v>39</v>
       </c>
       <c r="F13" s="1"/>
-      <c r="G13" s="21"/>
+      <c r="G13" s="22"/>
       <c r="H13" s="17"/>
     </row>
     <row r="14" spans="1:8" ht="48">
@@ -1150,7 +1158,7 @@
         <v>44</v>
       </c>
       <c r="F15" s="1"/>
-      <c r="G15" s="21"/>
+      <c r="G15" s="22"/>
       <c r="H15" s="17"/>
     </row>
     <row r="16" spans="1:8" ht="48">
@@ -1192,7 +1200,7 @@
         <v>49</v>
       </c>
       <c r="F17" s="1"/>
-      <c r="G17" s="21"/>
+      <c r="G17" s="22"/>
       <c r="H17" s="17"/>
     </row>
     <row r="18" spans="1:8" ht="48">
@@ -1234,7 +1242,7 @@
         <v>54</v>
       </c>
       <c r="F19" s="1"/>
-      <c r="G19" s="21"/>
+      <c r="G19" s="22"/>
       <c r="H19" s="17"/>
     </row>
     <row r="20" spans="1:8" ht="48">
@@ -1438,6 +1446,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010086172CFAA5FCEC4EBA8519FEE259A6B4" ma:contentTypeVersion="3" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2cf875f61f947313d43db5494becd2b8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="34ab6044-38b2-4dc7-97bb-2eb507f60812" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2e11831833257d99d0be17644557580d" ns2:_="">
     <xsd:import namespace="34ab6044-38b2-4dc7-97bb-2eb507f60812"/>
@@ -1575,20 +1589,14 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{95C7F316-54F6-4CFB-856D-9AD09D022CA2}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{20FD2E1A-4E2B-4A48-92AF-F21AB94E806B}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{291DE61A-00D2-4874-9EE9-2262838A2644}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{291DE61A-00D2-4874-9EE9-2262838A2644}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{20FD2E1A-4E2B-4A48-92AF-F21AB94E806B}"/>
 </file>
</xml_diff>